<commit_message>
Added Analysis of Algorithms.pdf
</commit_message>
<xml_diff>
--- a/lectures/Logarithms.xlsx
+++ b/lectures/Logarithms.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saqibali/Documents/git/algo-cs503/lectures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saqibali/Documents/git/bs-algo/lectures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92A733C-9B89-524C-B0DD-9BEE000E4742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8CCC95-65E3-9D42-B94E-6E419504F792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14820" xr2:uid="{7247F942-492A-5742-B340-6CA18B032E0C}"/>
+    <workbookView xWindow="3020" yWindow="520" windowWidth="25440" windowHeight="14640" activeTab="1" xr2:uid="{7247F942-492A-5742-B340-6CA18B032E0C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Log" sheetId="1" r:id="rId1"/>
+    <sheet name="Line" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>log base 10</t>
   </si>
@@ -103,12 +104,51 @@
   </si>
   <si>
     <t>depth</t>
+  </si>
+  <si>
+    <t>Problem Size (N)</t>
+  </si>
+  <si>
+    <t>Running Time</t>
+  </si>
+  <si>
+    <t>Slope of line</t>
+  </si>
+  <si>
+    <t>y Intercept</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Suppose that you make the following observations of the running time T(n)T(n)T(n) (in seconds) of a program as a function of the input size nnn. Which of the following functions best models the running time T(n)T(n)T(n)?</t>
+  </si>
+  <si>
+    <t>Problem Size</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predecited </t>
+  </si>
+  <si>
+    <t>log ratio</t>
+  </si>
+  <si>
+    <t>Log</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -153,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,6 +213,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,6 +234,1719 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.2494064118563026E-2"/>
+          <c:y val="0.16245370370370371"/>
+          <c:w val="0.9155301837270341"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Line!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Running Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Line!$A$4:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Line!$B$4:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-BAB0-EB4C-9C54-F7B1EFE92BA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="10314576"/>
+        <c:axId val="10403456"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="10314576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10403456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="10403456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10314576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Line!$E$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Running Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Line!$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Problem Size (N)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Line!$E$21:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="2">
+                  <c:v>-3.3219280948873622</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.32192809488736229</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6780719051126378</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6752513860502596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-969C-1749-8761-00CB537B9B30}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1761024"/>
+        <c:axId val="11258448"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1761024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11258448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="11258448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1761024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -234,6 +1993,83 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDCEFCDB-8D83-A241-AD4E-788137D500AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{026236C7-CA01-D842-9652-35C3C30BD210}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -538,7 +2374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC0B37C-B8FC-CB47-9895-42901F563E43}">
   <dimension ref="B5:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -1035,4 +2871,529 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9532625-F08E-E647-B84B-3BBD7A7A920E}">
+  <dimension ref="A3:E61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>250</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>500</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>4000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>51.1</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>16000</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>250</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21">
+        <f>LOG(A21,2)</f>
+        <v>7.965784284662087</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>500</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22">
+        <f t="shared" ref="D22:D27" si="0">LOG(A22,2)</f>
+        <v>8.965784284662087</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1000</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>9.965784284662087</v>
+      </c>
+      <c r="E23">
+        <f>LOG(B23,2)</f>
+        <v>-3.3219280948873622</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2000</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>10.965784284662087</v>
+      </c>
+      <c r="E24">
+        <f>LOG(B24,2)</f>
+        <v>-0.32192809488736229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>4000</v>
+      </c>
+      <c r="B25" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>11.965784284662087</v>
+      </c>
+      <c r="E25">
+        <f>LOG(B25,2)</f>
+        <v>2.6780719051126378</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>8000</v>
+      </c>
+      <c r="B26" s="1">
+        <v>51.1</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>12.965784284662087</v>
+      </c>
+      <c r="E26">
+        <f>LOG(B26,2)</f>
+        <v>5.6752513860502596</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>16000</v>
+      </c>
+      <c r="B27" s="8">
+        <f>B31*POWER(A27,B29)</f>
+        <v>409.59999999999985</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>13.965784284662087</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="10">
+        <f>(E24-E23)/(D24-D23)</f>
+        <v>3</v>
+      </c>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="5">
+        <f>E24-B29*D24</f>
+        <v>-33.219280948873624</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <f>POWER(2,B30)</f>
+        <v>9.9999999999999965E-11</v>
+      </c>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>250</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>500</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1000</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="D38" s="1">
+        <f>LOG(C38,2)</f>
+        <v>2.2630344058337939</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2000</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C39" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" ref="D39:D41" si="1">LOG(C39,2)</f>
+        <v>2.7865963618908069</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>4000</v>
+      </c>
+      <c r="B40" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="C40" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9448584458075393</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>8000</v>
+      </c>
+      <c r="B41" s="1">
+        <v>51.1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>8</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="5"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1">
+        <f>LOG(A51,2)</f>
+        <v>9.965784284662087</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" ref="C52:C57" si="2">LOG(A52,2)</f>
+        <v>10.965784284662087</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>4000</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="2"/>
+        <v>11.965784284662087</v>
+      </c>
+      <c r="D53">
+        <f>LOG(B53,2)</f>
+        <v>-3.3219280948873622</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>8000</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="2"/>
+        <v>12.965784284662087</v>
+      </c>
+      <c r="D54">
+        <f t="shared" ref="D54:D57" si="3">LOG(B54,2)</f>
+        <v>-1.7369655941662063</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>16000</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="2"/>
+        <v>13.965784284662087</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="3"/>
+        <v>0.37851162325372983</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>32000</v>
+      </c>
+      <c r="B56" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" si="2"/>
+        <v>14.965784284662087</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="3"/>
+        <v>2.3504972470841334</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>64000</v>
+      </c>
+      <c r="B57" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="C57" s="1">
+        <f t="shared" si="2"/>
+        <v>15.965784284662089</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="3"/>
+        <v>4.3575520046180838</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60">
+        <f>(D56-D55)/(C56-C55)</f>
+        <v>1.9719856238304037</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61">
+        <f>B57/POWER(A57,2)</f>
+        <v>5.0048828125000001E-9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A44:D48"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>